<commit_message>
smaller updated of presentation
</commit_message>
<xml_diff>
--- a/analyses Oli/Within and between tables.xlsx
+++ b/analyses Oli/Within and between tables.xlsx
@@ -406,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -541,6 +541,7 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -844,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:S143"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H67" sqref="H67:K79"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="E88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O100" sqref="O100:R108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2649,12 +2650,12 @@
       </c>
       <c r="J99" s="5"/>
       <c r="K99" s="5"/>
-      <c r="O99" s="21" t="s">
+      <c r="O99" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="P99" s="2"/>
-    </row>
-    <row r="100" spans="1:18" ht="31.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P99" s="37"/>
+    </row>
+    <row r="100" spans="1:18" ht="32.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
         <v>15</v>
       </c>
@@ -2678,14 +2679,14 @@
       <c r="K100" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="O100" s="3" t="s">
+      <c r="O100" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="P100" s="8" t="s">
+      <c r="P100" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="Q100" s="5"/>
-      <c r="R100" s="5"/>
+      <c r="Q100" s="27"/>
+      <c r="R100" s="27"/>
     </row>
     <row r="101" spans="1:18" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="10"/>
@@ -2731,7 +2732,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="102" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>16</v>
       </c>
@@ -2788,7 +2789,7 @@
         <v>-3.6656985222950809</v>
       </c>
     </row>
-    <row r="103" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>17</v>
       </c>
@@ -2845,7 +2846,7 @@
         <v>1.1911435783453665</v>
       </c>
     </row>
-    <row r="104" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>21</v>
       </c>
@@ -2902,7 +2903,7 @@
         <v>0.21345256719455125</v>
       </c>
     </row>
-    <row r="105" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>18</v>
       </c>
@@ -2959,7 +2960,7 @@
         <v>-0.28935248714732198</v>
       </c>
     </row>
-    <row r="106" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>20</v>
       </c>
@@ -3016,7 +3017,7 @@
         <v>1.7038121287396404</v>
       </c>
     </row>
-    <row r="107" spans="1:18" ht="54" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>19</v>
       </c>
@@ -3066,7 +3067,7 @@
         <v>0.32510973772476959</v>
       </c>
     </row>
-    <row r="108" spans="1:18" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="23" t="s">
         <v>27</v>
       </c>

</xml_diff>